<commit_message>
Cambios en la rubrica de jesus
</commit_message>
<xml_diff>
--- a/docs/Rubrica Trabajo en grupo.xlsx
+++ b/docs/Rubrica Trabajo en grupo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/n4xo/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cestino\Documents\ABD\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EEE8E91-1137-C443-A098-C2FDD51BA122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51ABEC63-DD92-4C16-B56A-A5F9ED28986F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="72">
   <si>
     <t>Miscelanea</t>
   </si>
@@ -240,6 +240,21 @@
   </si>
   <si>
     <t>Sí, select de la tabla en cuestión.</t>
+  </si>
+  <si>
+    <t>La carpeta Vistas de la base de datos, buscar con el nombre V_SALDOS</t>
+  </si>
+  <si>
+    <t>La carpeta Vistas de la base de datos, buscar con el nombre V_TARJETA_MENSUAL</t>
+  </si>
+  <si>
+    <t>La carpeta Vistas de la base de datos, buscar con el nombre V_PAGOS_PENDIENTES</t>
+  </si>
+  <si>
+    <t>La carpeta Paquetes de la base de datos, buscar con el nombre PK_GESTION_CUENTAS</t>
+  </si>
+  <si>
+    <t>La carpeta Paquetes de la base de datos, buscar con el nombre PK_GESTION_CLIENTES</t>
   </si>
 </sst>
 </file>
@@ -455,24 +470,24 @@
     </xf>
   </cellXfs>
   <cellStyles count="19">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -763,20 +778,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.83203125" style="8" customWidth="1"/>
-    <col min="2" max="2" width="23.83203125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="57.5" style="8" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" customWidth="1"/>
-    <col min="5" max="5" width="51.5" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" style="8" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" style="8" customWidth="1"/>
+    <col min="3" max="3" width="57.42578125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1"/>
+    <col min="5" max="5" width="51.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="23" customFormat="1" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="23" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>4</v>
       </c>
@@ -785,7 +800,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="22" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" s="22" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
         <v>57</v>
       </c>
@@ -804,7 +819,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -813,7 +828,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
@@ -827,7 +842,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5"/>
       <c r="B5" s="5" t="s">
         <v>46</v>
@@ -836,7 +851,7 @@
       <c r="D5" s="5"/>
       <c r="E5" s="8"/>
     </row>
-    <row r="6" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -855,7 +870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A7"/>
       <c r="C7" s="7" t="s">
         <v>16</v>
@@ -871,7 +886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A8"/>
       <c r="C8" s="8" t="s">
         <v>17</v>
@@ -887,7 +902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A9"/>
       <c r="C9" s="8" t="s">
         <v>54</v>
@@ -902,7 +917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <f>A6+1</f>
         <v>2</v>
@@ -913,7 +928,7 @@
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
     </row>
-    <row r="11" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11"/>
       <c r="C11" s="8" t="s">
         <v>18</v>
@@ -921,13 +936,15 @@
       <c r="D11" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="8"/>
+      <c r="E11" s="8" t="s">
+        <v>67</v>
+      </c>
       <c r="F11">
         <f>IF(D11="NO",0,1)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A12"/>
       <c r="C12" s="8" t="s">
         <v>19</v>
@@ -935,13 +952,15 @@
       <c r="D12" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="8"/>
+      <c r="E12" s="8" t="s">
+        <v>68</v>
+      </c>
       <c r="F12">
         <f t="shared" ref="F12:F13" si="0">IF(D12="NO",0,1)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A13"/>
       <c r="C13" s="8" t="s">
         <v>20</v>
@@ -949,13 +968,15 @@
       <c r="D13" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="8"/>
+      <c r="E13" s="8" t="s">
+        <v>69</v>
+      </c>
       <c r="F13">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A14"/>
       <c r="C14" s="8" t="s">
         <v>53</v>
@@ -968,7 +989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <f>A10+1</f>
         <v>3</v>
@@ -979,20 +1000,22 @@
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
     </row>
-    <row r="16" spans="1:7" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="C16" s="11" t="s">
         <v>21</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="11"/>
+      <c r="E16" s="11" t="s">
+        <v>71</v>
+      </c>
       <c r="F16">
         <f>IF(D16="NO",0,1)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A17"/>
       <c r="C17" s="6" t="s">
         <v>22</v>
@@ -1000,19 +1023,21 @@
       <c r="D17" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E17" s="8"/>
+      <c r="E17" s="8" t="s">
+        <v>70</v>
+      </c>
       <c r="F17">
         <f>IF(D17="NO",0,1)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
       <c r="E18" s="8"/>
     </row>
-    <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <f>A15+1</f>
         <v>4</v>
@@ -1024,7 +1049,7 @@
       <c r="D19" s="6"/>
       <c r="E19" s="8"/>
     </row>
-    <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20"/>
       <c r="C20" s="6" t="s">
         <v>15</v>
@@ -1038,14 +1063,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
       <c r="E21" s="8"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <f>A19+1</f>
         <v>5</v>
@@ -1056,7 +1081,7 @@
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
     </row>
-    <row r="23" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23"/>
       <c r="C23" s="8" t="s">
         <v>25</v>
@@ -1070,17 +1095,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24"/>
       <c r="D24" s="6"/>
       <c r="E24" s="8"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25"/>
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>5</v>
       </c>
@@ -1090,7 +1115,7 @@
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
     </row>
-    <row r="27" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27"/>
       <c r="C27" s="8" t="s">
         <v>27</v>
@@ -1100,12 +1125,12 @@
       </c>
       <c r="E27" s="8"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28"/>
       <c r="D28" s="6"/>
       <c r="E28" s="8"/>
     </row>
-    <row r="29" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <f>A26+1</f>
         <v>6</v>
@@ -1114,7 +1139,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A30"/>
       <c r="B30" s="1"/>
       <c r="C30" s="8" t="s">
@@ -1129,7 +1154,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <f>A29+1</f>
         <v>7</v>
@@ -1140,7 +1165,7 @@
       <c r="D31" s="6"/>
       <c r="E31" s="8"/>
     </row>
-    <row r="32" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32"/>
       <c r="B32" s="1"/>
       <c r="C32" s="8" t="s">
@@ -1155,13 +1180,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33"/>
       <c r="B33" s="1"/>
       <c r="D33" s="6"/>
       <c r="E33" s="8"/>
     </row>
-    <row r="34" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <f>A31+1</f>
         <v>8</v>
@@ -1178,19 +1203,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B35" s="13"/>
       <c r="C35" s="13"/>
       <c r="D35" s="13"/>
       <c r="E35" s="13"/>
     </row>
-    <row r="36" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B36" s="16"/>
       <c r="C36" s="16"/>
       <c r="D36" s="16"/>
       <c r="E36" s="16"/>
     </row>
-    <row r="37" spans="1:6" s="17" customFormat="1" ht="24" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" s="17" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B37" s="18" t="s">
         <v>10</v>
       </c>
@@ -1202,7 +1227,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="1:6" s="14" customFormat="1" ht="24" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" s="14" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B38" s="21" t="s">
         <v>11</v>
       </c>
@@ -1210,7 +1235,7 @@
       <c r="D38" s="13"/>
       <c r="E38" s="13"/>
     </row>
-    <row r="39" spans="1:6" s="17" customFormat="1" ht="24" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" s="17" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B39" s="18" t="s">
         <v>12</v>
       </c>
@@ -1218,19 +1243,19 @@
       <c r="D39" s="16"/>
       <c r="E39" s="16"/>
     </row>
-    <row r="40" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B40" s="16"/>
       <c r="C40" s="16"/>
       <c r="D40" s="16"/>
       <c r="E40" s="16"/>
     </row>
-    <row r="41" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B41" s="16"/>
       <c r="C41" s="16"/>
       <c r="D41" s="16"/>
       <c r="E41" s="16"/>
     </row>
-    <row r="42" spans="1:6" s="17" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="17">
         <v>1</v>
       </c>
@@ -1241,7 +1266,7 @@
       <c r="D42" s="16"/>
       <c r="E42" s="16"/>
     </row>
-    <row r="43" spans="1:6" s="17" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B43" s="16"/>
       <c r="C43" s="16" t="s">
         <v>42</v>
@@ -1255,7 +1280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:6" s="17" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B44" s="16"/>
       <c r="C44" s="16" t="s">
         <v>43</v>
@@ -1269,7 +1294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45"/>
       <c r="C45" s="8" t="s">
         <v>26</v>
@@ -1283,13 +1308,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B46" s="16"/>
       <c r="C46" s="16"/>
       <c r="D46" s="16"/>
       <c r="E46" s="16"/>
     </row>
-    <row r="47" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="17">
         <f>A42+1</f>
         <v>2</v>
@@ -1302,7 +1327,7 @@
       <c r="E47" s="8"/>
       <c r="F47"/>
     </row>
-    <row r="48" spans="1:6" s="17" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" s="17" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B48" s="8"/>
       <c r="C48" s="8" t="s">
         <v>30</v>
@@ -1316,7 +1341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:6" s="17" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B49" s="8"/>
       <c r="C49" s="9" t="s">
         <v>31</v>
@@ -1330,7 +1355,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
         <f>A47+1</f>
         <v>3</v>
@@ -1341,7 +1366,7 @@
       <c r="D50" s="8"/>
       <c r="E50" s="8"/>
     </row>
-    <row r="51" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51"/>
       <c r="C51" s="8" t="s">
         <v>33</v>
@@ -1355,7 +1380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52"/>
       <c r="C52" s="8" t="s">
         <v>34</v>
@@ -1369,7 +1394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A53"/>
       <c r="C53" s="8" t="s">
         <v>35</v>
@@ -1379,7 +1404,7 @@
       </c>
       <c r="E53" s="8"/>
     </row>
-    <row r="54" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54"/>
       <c r="C54" s="8" t="s">
         <v>36</v>
@@ -1393,7 +1418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55"/>
       <c r="C55" s="8" t="s">
         <v>37</v>
@@ -1407,7 +1432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56"/>
       <c r="C56" s="8" t="s">
         <v>38</v>
@@ -1421,7 +1446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57"/>
       <c r="C57" s="8" t="s">
         <v>39</v>
@@ -1435,7 +1460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58"/>
       <c r="C58" s="8" t="s">
         <v>52</v>
@@ -1449,7 +1474,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59">
         <f>A50+1</f>
         <v>4</v>
@@ -1460,7 +1485,7 @@
       <c r="D59" s="8"/>
       <c r="E59" s="8"/>
     </row>
-    <row r="60" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A60"/>
       <c r="C60" s="8" t="s">
         <v>40</v>
@@ -1474,13 +1499,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61"/>
       <c r="B61" s="1"/>
       <c r="D61" s="8"/>
       <c r="E61" s="8"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62">
         <f>A59+1</f>
         <v>5</v>
@@ -1492,7 +1517,7 @@
       <c r="D62" s="4"/>
       <c r="E62" s="8"/>
     </row>
-    <row r="63" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A63"/>
       <c r="C63" s="8" t="s">
         <v>1</v>
@@ -1506,7 +1531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A64"/>
       <c r="C64" s="8" t="s">
         <v>41</v>
@@ -1520,7 +1545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="3:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="65" spans="3:6" ht="30" x14ac:dyDescent="0.25">
       <c r="C65" s="8" t="s">
         <v>55</v>
       </c>
@@ -1531,7 +1556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="3:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="66" spans="3:6" ht="30" x14ac:dyDescent="0.25">
       <c r="C66" s="8" t="s">
         <v>56</v>
       </c>
@@ -1575,22 +1600,22 @@
       <selection sqref="A1:A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>

</xml_diff>